<commit_message>
replace examples files for demo
</commit_message>
<xml_diff>
--- a/Challenge Part 1/Example_list_judges.xlsx
+++ b/Challenge Part 1/Example_list_judges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28602"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\prufesooor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sumailsyr-my.sharepoint.com/personal/rpal03_syr_edu/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC910C3-675B-44AD-87B1-8E0A142F047A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{21C4D955-71E6-4396-8A7A-125F62DB3098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E5B66F6D-C56A-4246-AA2F-7D443289F214}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E5B66F6D-C56A-4246-AA2F-7D443289F214}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>Judge</t>
   </si>
@@ -171,7 +171,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,13 +189,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -219,11 +212,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,15 +550,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825F5099-6D36-0843-8EF7-DDC1AB7C9624}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +576,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -602,7 +594,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -620,7 +612,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -638,7 +630,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -656,7 +648,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -674,7 +666,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -692,7 +684,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -710,7 +702,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -728,7 +720,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -746,7 +738,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -764,124 +756,133 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="3">
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="3" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E17" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="1">
         <v>1</v>
       </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="E21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>